<commit_message>
US202 & 201, added additional attributes with some mock data. Updated source for where this information can be found and looked for alternative ways to find this info.
Former-commit-id: 97744c606e2ad489703d37f45b923d058d314a58
</commit_message>
<xml_diff>
--- a/imdb_papers/Attributes.xlsx
+++ b/imdb_papers/Attributes.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\irondb\imdb_papers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{032E6C43-E619-43D4-8DD6-3018D7BC9A39}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>entry_id</t>
   </si>
@@ -43,9 +52,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Published Date</t>
-  </si>
-  <si>
     <t>inserted_date</t>
   </si>
   <si>
@@ -61,9 +67,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
     <t>IAB</t>
   </si>
   <si>
@@ -95,26 +98,112 @@
   </si>
   <si>
     <t>DOCUMENT</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Journal Name</t>
+  </si>
+  <si>
+    <t>Page #</t>
+  </si>
+  <si>
+    <t>Published Year</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>Bahjoi</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification and origin of lAB and IIICD iron meteorites </t>
+  </si>
+  <si>
+    <t>Byeon-Gak Choi, Xinwei Ouyang, John T Wasson</t>
+  </si>
+  <si>
+    <t>Geochimica et Cosmochimica Acta</t>
+  </si>
+  <si>
+    <t>Journal/Issue #</t>
+  </si>
+  <si>
+    <t>0016-7037(94)00384-X</t>
+  </si>
+  <si>
+    <t>DOCUMENT/DOI</t>
+  </si>
+  <si>
+    <t>Chemical classification of iron meteorites—IX. A new group (IIF), revision of IAB and IIICD, and data on 57 additional irons</t>
+  </si>
+  <si>
+    <t>Alfred Kracher, John Willis, John T Wasson</t>
+  </si>
+  <si>
+    <t>Alt Bela</t>
+  </si>
+  <si>
+    <t>IID</t>
+  </si>
+  <si>
+    <t>Ni, Ga</t>
+  </si>
+  <si>
+    <t>Ge</t>
+  </si>
+  <si>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>NMW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/0016-7037(80)90259-8} </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -124,66 +213,397 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AJ1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.29"/>
-    <col customWidth="1" min="2" max="2" width="15.43"/>
-    <col customWidth="1" min="3" max="3" width="21.29"/>
-    <col customWidth="1" min="5" max="5" width="24.57"/>
-    <col customWidth="1" min="6" max="6" width="21.29"/>
-    <col customWidth="1" min="7" max="7" width="26.71"/>
-    <col customWidth="1" min="8" max="8" width="17.0"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -216,27 +636,35 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -248,3100 +676,3183 @@
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+    </row>
+    <row r="2" spans="1:36" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="I2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="8">
+        <v>595</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="9">
+        <v>59.3</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1995</v>
+      </c>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="U2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:36" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3">
+        <v>774</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3">
+        <v>44</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3">
+        <v>1980</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4">
+    </row>
+    <row r="4" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>23</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6"/>
     </row>
-    <row r="19">
+    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6"/>
     </row>
-    <row r="20">
+    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
     </row>
-    <row r="21">
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
     </row>
-    <row r="22">
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6"/>
     </row>
-    <row r="23">
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6"/>
     </row>
-    <row r="24">
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
     </row>
-    <row r="26">
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
     </row>
-    <row r="27">
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
     </row>
-    <row r="32">
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6"/>
     </row>
-    <row r="33">
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
     </row>
-    <row r="34">
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
     </row>
-    <row r="35">
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
     </row>
-    <row r="36">
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6"/>
     </row>
-    <row r="37">
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
     </row>
-    <row r="38">
+    <row r="38" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B38" s="6"/>
     </row>
-    <row r="39">
+    <row r="39" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B39" s="6"/>
     </row>
-    <row r="40">
+    <row r="40" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B40" s="6"/>
     </row>
-    <row r="41">
+    <row r="41" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B41" s="6"/>
     </row>
-    <row r="42">
+    <row r="42" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B42" s="6"/>
     </row>
-    <row r="43">
+    <row r="43" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B43" s="6"/>
     </row>
-    <row r="44">
+    <row r="44" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B44" s="6"/>
     </row>
-    <row r="45">
+    <row r="45" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
     </row>
-    <row r="46">
+    <row r="46" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B46" s="6"/>
     </row>
-    <row r="47">
+    <row r="47" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B47" s="6"/>
     </row>
-    <row r="48">
+    <row r="48" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
     </row>
-    <row r="49">
+    <row r="49" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B49" s="6"/>
     </row>
-    <row r="50">
+    <row r="50" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B50" s="6"/>
     </row>
-    <row r="51">
+    <row r="51" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="6"/>
     </row>
-    <row r="52">
+    <row r="52" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="6"/>
     </row>
-    <row r="53">
+    <row r="53" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B53" s="6"/>
     </row>
-    <row r="54">
+    <row r="54" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B54" s="6"/>
     </row>
-    <row r="55">
+    <row r="55" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B55" s="6"/>
     </row>
-    <row r="56">
+    <row r="56" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B56" s="6"/>
     </row>
-    <row r="57">
+    <row r="57" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B57" s="6"/>
     </row>
-    <row r="58">
+    <row r="58" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B58" s="6"/>
     </row>
-    <row r="59">
+    <row r="59" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B59" s="6"/>
     </row>
-    <row r="60">
+    <row r="60" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="6"/>
     </row>
-    <row r="61">
+    <row r="61" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B61" s="6"/>
     </row>
-    <row r="62">
+    <row r="62" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B62" s="6"/>
     </row>
-    <row r="63">
+    <row r="63" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="6"/>
     </row>
-    <row r="64">
+    <row r="64" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="6"/>
     </row>
-    <row r="65">
+    <row r="65" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B65" s="6"/>
     </row>
-    <row r="66">
+    <row r="66" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B66" s="6"/>
     </row>
-    <row r="67">
+    <row r="67" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B67" s="6"/>
     </row>
-    <row r="68">
+    <row r="68" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B68" s="6"/>
     </row>
-    <row r="69">
+    <row r="69" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B69" s="6"/>
     </row>
-    <row r="70">
+    <row r="70" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B70" s="6"/>
     </row>
-    <row r="71">
+    <row r="71" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B71" s="6"/>
     </row>
-    <row r="72">
+    <row r="72" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B72" s="6"/>
     </row>
-    <row r="73">
+    <row r="73" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73" s="6"/>
     </row>
-    <row r="74">
+    <row r="74" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74" s="6"/>
     </row>
-    <row r="75">
+    <row r="75" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75" s="6"/>
     </row>
-    <row r="76">
+    <row r="76" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76" s="6"/>
     </row>
-    <row r="77">
+    <row r="77" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77" s="6"/>
     </row>
-    <row r="78">
+    <row r="78" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78" s="6"/>
     </row>
-    <row r="79">
+    <row r="79" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79" s="6"/>
     </row>
-    <row r="80">
+    <row r="80" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="6"/>
     </row>
-    <row r="81">
+    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81" s="6"/>
     </row>
-    <row r="82">
+    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B82" s="6"/>
     </row>
-    <row r="83">
+    <row r="83" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B83" s="6"/>
     </row>
-    <row r="84">
+    <row r="84" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B84" s="6"/>
     </row>
-    <row r="85">
+    <row r="85" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B85" s="6"/>
     </row>
-    <row r="86">
+    <row r="86" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B86" s="6"/>
     </row>
-    <row r="87">
+    <row r="87" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B87" s="6"/>
     </row>
-    <row r="88">
+    <row r="88" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B88" s="6"/>
     </row>
-    <row r="89">
+    <row r="89" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B89" s="6"/>
     </row>
-    <row r="90">
+    <row r="90" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B90" s="6"/>
     </row>
-    <row r="91">
+    <row r="91" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B91" s="6"/>
     </row>
-    <row r="92">
+    <row r="92" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B92" s="6"/>
     </row>
-    <row r="93">
+    <row r="93" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B93" s="6"/>
     </row>
-    <row r="94">
+    <row r="94" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B94" s="6"/>
     </row>
-    <row r="95">
+    <row r="95" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B95" s="6"/>
     </row>
-    <row r="96">
+    <row r="96" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B96" s="6"/>
     </row>
-    <row r="97">
+    <row r="97" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B97" s="6"/>
     </row>
-    <row r="98">
+    <row r="98" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B98" s="6"/>
     </row>
-    <row r="99">
+    <row r="99" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B99" s="6"/>
     </row>
-    <row r="100">
+    <row r="100" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B100" s="6"/>
     </row>
-    <row r="101">
+    <row r="101" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B101" s="6"/>
     </row>
-    <row r="102">
+    <row r="102" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B102" s="6"/>
     </row>
-    <row r="103">
+    <row r="103" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B103" s="6"/>
     </row>
-    <row r="104">
+    <row r="104" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B104" s="6"/>
     </row>
-    <row r="105">
+    <row r="105" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B105" s="6"/>
     </row>
-    <row r="106">
+    <row r="106" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B106" s="6"/>
     </row>
-    <row r="107">
+    <row r="107" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B107" s="6"/>
     </row>
-    <row r="108">
+    <row r="108" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B108" s="6"/>
     </row>
-    <row r="109">
+    <row r="109" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B109" s="6"/>
     </row>
-    <row r="110">
+    <row r="110" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B110" s="6"/>
     </row>
-    <row r="111">
+    <row r="111" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B111" s="6"/>
     </row>
-    <row r="112">
+    <row r="112" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B112" s="6"/>
     </row>
-    <row r="113">
+    <row r="113" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B113" s="6"/>
     </row>
-    <row r="114">
+    <row r="114" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B114" s="6"/>
     </row>
-    <row r="115">
+    <row r="115" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B115" s="6"/>
     </row>
-    <row r="116">
+    <row r="116" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B116" s="6"/>
     </row>
-    <row r="117">
+    <row r="117" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B117" s="6"/>
     </row>
-    <row r="118">
+    <row r="118" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B118" s="6"/>
     </row>
-    <row r="119">
+    <row r="119" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B119" s="6"/>
     </row>
-    <row r="120">
+    <row r="120" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B120" s="6"/>
     </row>
-    <row r="121">
+    <row r="121" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B121" s="6"/>
     </row>
-    <row r="122">
+    <row r="122" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B122" s="6"/>
     </row>
-    <row r="123">
+    <row r="123" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B123" s="6"/>
     </row>
-    <row r="124">
+    <row r="124" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B124" s="6"/>
     </row>
-    <row r="125">
+    <row r="125" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B125" s="6"/>
     </row>
-    <row r="126">
+    <row r="126" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B126" s="6"/>
     </row>
-    <row r="127">
+    <row r="127" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B127" s="6"/>
     </row>
-    <row r="128">
+    <row r="128" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B128" s="6"/>
     </row>
-    <row r="129">
+    <row r="129" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B129" s="6"/>
     </row>
-    <row r="130">
+    <row r="130" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B130" s="6"/>
     </row>
-    <row r="131">
+    <row r="131" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B131" s="6"/>
     </row>
-    <row r="132">
+    <row r="132" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B132" s="6"/>
     </row>
-    <row r="133">
+    <row r="133" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B133" s="6"/>
     </row>
-    <row r="134">
+    <row r="134" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B134" s="6"/>
     </row>
-    <row r="135">
+    <row r="135" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B135" s="6"/>
     </row>
-    <row r="136">
+    <row r="136" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B136" s="6"/>
     </row>
-    <row r="137">
+    <row r="137" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B137" s="6"/>
     </row>
-    <row r="138">
+    <row r="138" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B138" s="6"/>
     </row>
-    <row r="139">
+    <row r="139" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B139" s="6"/>
     </row>
-    <row r="140">
+    <row r="140" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B140" s="6"/>
     </row>
-    <row r="141">
+    <row r="141" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B141" s="6"/>
     </row>
-    <row r="142">
+    <row r="142" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B142" s="6"/>
     </row>
-    <row r="143">
+    <row r="143" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B143" s="6"/>
     </row>
-    <row r="144">
+    <row r="144" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B144" s="6"/>
     </row>
-    <row r="145">
+    <row r="145" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B145" s="6"/>
     </row>
-    <row r="146">
+    <row r="146" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B146" s="6"/>
     </row>
-    <row r="147">
+    <row r="147" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B147" s="6"/>
     </row>
-    <row r="148">
+    <row r="148" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B148" s="6"/>
     </row>
-    <row r="149">
+    <row r="149" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B149" s="6"/>
     </row>
-    <row r="150">
+    <row r="150" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B150" s="6"/>
     </row>
-    <row r="151">
+    <row r="151" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B151" s="6"/>
     </row>
-    <row r="152">
+    <row r="152" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B152" s="6"/>
     </row>
-    <row r="153">
+    <row r="153" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B153" s="6"/>
     </row>
-    <row r="154">
+    <row r="154" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B154" s="6"/>
     </row>
-    <row r="155">
+    <row r="155" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B155" s="6"/>
     </row>
-    <row r="156">
+    <row r="156" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B156" s="6"/>
     </row>
-    <row r="157">
+    <row r="157" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B157" s="6"/>
     </row>
-    <row r="158">
+    <row r="158" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B158" s="6"/>
     </row>
-    <row r="159">
+    <row r="159" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B159" s="6"/>
     </row>
-    <row r="160">
+    <row r="160" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B160" s="6"/>
     </row>
-    <row r="161">
+    <row r="161" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B161" s="6"/>
     </row>
-    <row r="162">
+    <row r="162" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B162" s="6"/>
     </row>
-    <row r="163">
+    <row r="163" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B163" s="6"/>
     </row>
-    <row r="164">
+    <row r="164" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B164" s="6"/>
     </row>
-    <row r="165">
+    <row r="165" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B165" s="6"/>
     </row>
-    <row r="166">
+    <row r="166" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B166" s="6"/>
     </row>
-    <row r="167">
+    <row r="167" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B167" s="6"/>
     </row>
-    <row r="168">
+    <row r="168" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B168" s="6"/>
     </row>
-    <row r="169">
+    <row r="169" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B169" s="6"/>
     </row>
-    <row r="170">
+    <row r="170" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B170" s="6"/>
     </row>
-    <row r="171">
+    <row r="171" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B171" s="6"/>
     </row>
-    <row r="172">
+    <row r="172" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B172" s="6"/>
     </row>
-    <row r="173">
+    <row r="173" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B173" s="6"/>
     </row>
-    <row r="174">
+    <row r="174" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B174" s="6"/>
     </row>
-    <row r="175">
+    <row r="175" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B175" s="6"/>
     </row>
-    <row r="176">
+    <row r="176" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B176" s="6"/>
     </row>
-    <row r="177">
+    <row r="177" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178">
+    <row r="178" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179">
+    <row r="179" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180">
+    <row r="180" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181">
+    <row r="181" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182">
+    <row r="182" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183">
+    <row r="183" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184">
+    <row r="184" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185">
+    <row r="185" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186">
+    <row r="186" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187">
+    <row r="187" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188">
+    <row r="188" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189">
+    <row r="189" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190">
+    <row r="190" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191">
+    <row r="191" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192">
+    <row r="192" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193">
+    <row r="193" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194">
+    <row r="194" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195">
+    <row r="195" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196">
+    <row r="196" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197">
+    <row r="197" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198">
+    <row r="198" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199">
+    <row r="199" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200">
+    <row r="200" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201">
+    <row r="201" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202">
+    <row r="202" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203">
+    <row r="203" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204">
+    <row r="204" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205">
+    <row r="205" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206">
+    <row r="206" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207">
+    <row r="207" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208">
+    <row r="208" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209">
+    <row r="209" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210">
+    <row r="210" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211">
+    <row r="211" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B211" s="6"/>
     </row>
-    <row r="212">
+    <row r="212" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B212" s="6"/>
     </row>
-    <row r="213">
+    <row r="213" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B213" s="6"/>
     </row>
-    <row r="214">
+    <row r="214" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B214" s="6"/>
     </row>
-    <row r="215">
+    <row r="215" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B215" s="6"/>
     </row>
-    <row r="216">
+    <row r="216" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B216" s="6"/>
     </row>
-    <row r="217">
+    <row r="217" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B217" s="6"/>
     </row>
-    <row r="218">
+    <row r="218" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B218" s="6"/>
     </row>
-    <row r="219">
+    <row r="219" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B219" s="6"/>
     </row>
-    <row r="220">
+    <row r="220" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B220" s="6"/>
     </row>
-    <row r="221">
+    <row r="221" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B221" s="6"/>
     </row>
-    <row r="222">
+    <row r="222" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B222" s="6"/>
     </row>
-    <row r="223">
+    <row r="223" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B223" s="6"/>
     </row>
-    <row r="224">
+    <row r="224" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B224" s="6"/>
     </row>
-    <row r="225">
+    <row r="225" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B225" s="6"/>
     </row>
-    <row r="226">
+    <row r="226" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B226" s="6"/>
     </row>
-    <row r="227">
+    <row r="227" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B227" s="6"/>
     </row>
-    <row r="228">
+    <row r="228" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B228" s="6"/>
     </row>
-    <row r="229">
+    <row r="229" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B229" s="6"/>
     </row>
-    <row r="230">
+    <row r="230" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B230" s="6"/>
     </row>
-    <row r="231">
+    <row r="231" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B231" s="6"/>
     </row>
-    <row r="232">
+    <row r="232" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B232" s="6"/>
     </row>
-    <row r="233">
+    <row r="233" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B233" s="6"/>
     </row>
-    <row r="234">
+    <row r="234" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B234" s="6"/>
     </row>
-    <row r="235">
+    <row r="235" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B235" s="6"/>
     </row>
-    <row r="236">
+    <row r="236" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B236" s="6"/>
     </row>
-    <row r="237">
+    <row r="237" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B237" s="6"/>
     </row>
-    <row r="238">
+    <row r="238" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B238" s="6"/>
     </row>
-    <row r="239">
+    <row r="239" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B239" s="6"/>
     </row>
-    <row r="240">
+    <row r="240" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B240" s="6"/>
     </row>
-    <row r="241">
+    <row r="241" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B241" s="6"/>
     </row>
-    <row r="242">
+    <row r="242" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B242" s="6"/>
     </row>
-    <row r="243">
+    <row r="243" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B243" s="6"/>
     </row>
-    <row r="244">
+    <row r="244" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B244" s="6"/>
     </row>
-    <row r="245">
+    <row r="245" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B245" s="6"/>
     </row>
-    <row r="246">
+    <row r="246" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B246" s="6"/>
     </row>
-    <row r="247">
+    <row r="247" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B247" s="6"/>
     </row>
-    <row r="248">
+    <row r="248" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B248" s="6"/>
     </row>
-    <row r="249">
+    <row r="249" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B249" s="6"/>
     </row>
-    <row r="250">
+    <row r="250" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B250" s="6"/>
     </row>
-    <row r="251">
+    <row r="251" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B251" s="6"/>
     </row>
-    <row r="252">
+    <row r="252" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B252" s="6"/>
     </row>
-    <row r="253">
+    <row r="253" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B253" s="6"/>
     </row>
-    <row r="254">
+    <row r="254" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B254" s="6"/>
     </row>
-    <row r="255">
+    <row r="255" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B255" s="6"/>
     </row>
-    <row r="256">
+    <row r="256" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B256" s="6"/>
     </row>
-    <row r="257">
+    <row r="257" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B257" s="6"/>
     </row>
-    <row r="258">
+    <row r="258" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B258" s="6"/>
     </row>
-    <row r="259">
+    <row r="259" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B259" s="6"/>
     </row>
-    <row r="260">
+    <row r="260" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B260" s="6"/>
     </row>
-    <row r="261">
+    <row r="261" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B261" s="6"/>
     </row>
-    <row r="262">
+    <row r="262" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B262" s="6"/>
     </row>
-    <row r="263">
+    <row r="263" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B263" s="6"/>
     </row>
-    <row r="264">
+    <row r="264" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B264" s="6"/>
     </row>
-    <row r="265">
+    <row r="265" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B265" s="6"/>
     </row>
-    <row r="266">
+    <row r="266" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B266" s="6"/>
     </row>
-    <row r="267">
+    <row r="267" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B267" s="6"/>
     </row>
-    <row r="268">
+    <row r="268" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B268" s="6"/>
     </row>
-    <row r="269">
+    <row r="269" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B269" s="6"/>
     </row>
-    <row r="270">
+    <row r="270" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B270" s="6"/>
     </row>
-    <row r="271">
+    <row r="271" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B271" s="6"/>
     </row>
-    <row r="272">
+    <row r="272" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B272" s="6"/>
     </row>
-    <row r="273">
+    <row r="273" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B273" s="6"/>
     </row>
-    <row r="274">
+    <row r="274" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B274" s="6"/>
     </row>
-    <row r="275">
+    <row r="275" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B275" s="6"/>
     </row>
-    <row r="276">
+    <row r="276" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B276" s="6"/>
     </row>
-    <row r="277">
+    <row r="277" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B277" s="6"/>
     </row>
-    <row r="278">
+    <row r="278" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B278" s="6"/>
     </row>
-    <row r="279">
+    <row r="279" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B279" s="6"/>
     </row>
-    <row r="280">
+    <row r="280" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B280" s="6"/>
     </row>
-    <row r="281">
+    <row r="281" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B281" s="6"/>
     </row>
-    <row r="282">
+    <row r="282" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B282" s="6"/>
     </row>
-    <row r="283">
+    <row r="283" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B283" s="6"/>
     </row>
-    <row r="284">
+    <row r="284" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B284" s="6"/>
     </row>
-    <row r="285">
+    <row r="285" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B285" s="6"/>
     </row>
-    <row r="286">
+    <row r="286" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B286" s="6"/>
     </row>
-    <row r="287">
+    <row r="287" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B287" s="6"/>
     </row>
-    <row r="288">
+    <row r="288" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B288" s="6"/>
     </row>
-    <row r="289">
+    <row r="289" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B289" s="6"/>
     </row>
-    <row r="290">
+    <row r="290" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B290" s="6"/>
     </row>
-    <row r="291">
+    <row r="291" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B291" s="6"/>
     </row>
-    <row r="292">
+    <row r="292" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B292" s="6"/>
     </row>
-    <row r="293">
+    <row r="293" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B293" s="6"/>
     </row>
-    <row r="294">
+    <row r="294" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B294" s="6"/>
     </row>
-    <row r="295">
+    <row r="295" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B295" s="6"/>
     </row>
-    <row r="296">
+    <row r="296" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B296" s="6"/>
     </row>
-    <row r="297">
+    <row r="297" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B297" s="6"/>
     </row>
-    <row r="298">
+    <row r="298" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B298" s="6"/>
     </row>
-    <row r="299">
+    <row r="299" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B299" s="6"/>
     </row>
-    <row r="300">
+    <row r="300" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B300" s="6"/>
     </row>
-    <row r="301">
+    <row r="301" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B301" s="6"/>
     </row>
-    <row r="302">
+    <row r="302" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B302" s="6"/>
     </row>
-    <row r="303">
+    <row r="303" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B303" s="6"/>
     </row>
-    <row r="304">
+    <row r="304" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B304" s="6"/>
     </row>
-    <row r="305">
+    <row r="305" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B305" s="6"/>
     </row>
-    <row r="306">
+    <row r="306" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B306" s="6"/>
     </row>
-    <row r="307">
+    <row r="307" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B307" s="6"/>
     </row>
-    <row r="308">
+    <row r="308" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B308" s="6"/>
     </row>
-    <row r="309">
+    <row r="309" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B309" s="6"/>
     </row>
-    <row r="310">
+    <row r="310" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B310" s="6"/>
     </row>
-    <row r="311">
+    <row r="311" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B311" s="6"/>
     </row>
-    <row r="312">
+    <row r="312" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B312" s="6"/>
     </row>
-    <row r="313">
+    <row r="313" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B313" s="6"/>
     </row>
-    <row r="314">
+    <row r="314" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B314" s="6"/>
     </row>
-    <row r="315">
+    <row r="315" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B315" s="6"/>
     </row>
-    <row r="316">
+    <row r="316" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B316" s="6"/>
     </row>
-    <row r="317">
+    <row r="317" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B317" s="6"/>
     </row>
-    <row r="318">
+    <row r="318" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B318" s="6"/>
     </row>
-    <row r="319">
+    <row r="319" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B319" s="6"/>
     </row>
-    <row r="320">
+    <row r="320" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B320" s="6"/>
     </row>
-    <row r="321">
+    <row r="321" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B321" s="6"/>
     </row>
-    <row r="322">
+    <row r="322" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B322" s="6"/>
     </row>
-    <row r="323">
+    <row r="323" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B323" s="6"/>
     </row>
-    <row r="324">
+    <row r="324" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B324" s="6"/>
     </row>
-    <row r="325">
+    <row r="325" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B325" s="6"/>
     </row>
-    <row r="326">
+    <row r="326" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B326" s="6"/>
     </row>
-    <row r="327">
+    <row r="327" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B327" s="6"/>
     </row>
-    <row r="328">
+    <row r="328" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B328" s="6"/>
     </row>
-    <row r="329">
+    <row r="329" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B329" s="6"/>
     </row>
-    <row r="330">
+    <row r="330" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B330" s="6"/>
     </row>
-    <row r="331">
+    <row r="331" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B331" s="6"/>
     </row>
-    <row r="332">
+    <row r="332" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B332" s="6"/>
     </row>
-    <row r="333">
+    <row r="333" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B333" s="6"/>
     </row>
-    <row r="334">
+    <row r="334" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B334" s="6"/>
     </row>
-    <row r="335">
+    <row r="335" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B335" s="6"/>
     </row>
-    <row r="336">
+    <row r="336" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B336" s="6"/>
     </row>
-    <row r="337">
+    <row r="337" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B337" s="6"/>
     </row>
-    <row r="338">
+    <row r="338" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B338" s="6"/>
     </row>
-    <row r="339">
+    <row r="339" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B339" s="6"/>
     </row>
-    <row r="340">
+    <row r="340" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B340" s="6"/>
     </row>
-    <row r="341">
+    <row r="341" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B341" s="6"/>
     </row>
-    <row r="342">
+    <row r="342" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B342" s="6"/>
     </row>
-    <row r="343">
+    <row r="343" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B343" s="6"/>
     </row>
-    <row r="344">
+    <row r="344" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B344" s="6"/>
     </row>
-    <row r="345">
+    <row r="345" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B345" s="6"/>
     </row>
-    <row r="346">
+    <row r="346" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B346" s="6"/>
     </row>
-    <row r="347">
+    <row r="347" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B347" s="6"/>
     </row>
-    <row r="348">
+    <row r="348" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B348" s="6"/>
     </row>
-    <row r="349">
+    <row r="349" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B349" s="6"/>
     </row>
-    <row r="350">
+    <row r="350" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B350" s="6"/>
     </row>
-    <row r="351">
+    <row r="351" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B351" s="6"/>
     </row>
-    <row r="352">
+    <row r="352" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B352" s="6"/>
     </row>
-    <row r="353">
+    <row r="353" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B353" s="6"/>
     </row>
-    <row r="354">
+    <row r="354" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B354" s="6"/>
     </row>
-    <row r="355">
+    <row r="355" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B355" s="6"/>
     </row>
-    <row r="356">
+    <row r="356" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B356" s="6"/>
     </row>
-    <row r="357">
+    <row r="357" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B357" s="6"/>
     </row>
-    <row r="358">
+    <row r="358" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B358" s="6"/>
     </row>
-    <row r="359">
+    <row r="359" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B359" s="6"/>
     </row>
-    <row r="360">
+    <row r="360" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B360" s="6"/>
     </row>
-    <row r="361">
+    <row r="361" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B361" s="6"/>
     </row>
-    <row r="362">
+    <row r="362" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B362" s="6"/>
     </row>
-    <row r="363">
+    <row r="363" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B363" s="6"/>
     </row>
-    <row r="364">
+    <row r="364" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B364" s="6"/>
     </row>
-    <row r="365">
+    <row r="365" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B365" s="6"/>
     </row>
-    <row r="366">
+    <row r="366" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B366" s="6"/>
     </row>
-    <row r="367">
+    <row r="367" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B367" s="6"/>
     </row>
-    <row r="368">
+    <row r="368" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B368" s="6"/>
     </row>
-    <row r="369">
+    <row r="369" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B369" s="6"/>
     </row>
-    <row r="370">
+    <row r="370" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B370" s="6"/>
     </row>
-    <row r="371">
+    <row r="371" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B371" s="6"/>
     </row>
-    <row r="372">
+    <row r="372" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B372" s="6"/>
     </row>
-    <row r="373">
+    <row r="373" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B373" s="6"/>
     </row>
-    <row r="374">
+    <row r="374" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B374" s="6"/>
     </row>
-    <row r="375">
+    <row r="375" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B375" s="6"/>
     </row>
-    <row r="376">
+    <row r="376" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B376" s="6"/>
     </row>
-    <row r="377">
+    <row r="377" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B377" s="6"/>
     </row>
-    <row r="378">
+    <row r="378" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B378" s="6"/>
     </row>
-    <row r="379">
+    <row r="379" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B379" s="6"/>
     </row>
-    <row r="380">
+    <row r="380" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B380" s="6"/>
     </row>
-    <row r="381">
+    <row r="381" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B381" s="6"/>
     </row>
-    <row r="382">
+    <row r="382" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B382" s="6"/>
     </row>
-    <row r="383">
+    <row r="383" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B383" s="6"/>
     </row>
-    <row r="384">
+    <row r="384" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B384" s="6"/>
     </row>
-    <row r="385">
+    <row r="385" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B385" s="6"/>
     </row>
-    <row r="386">
+    <row r="386" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B386" s="6"/>
     </row>
-    <row r="387">
+    <row r="387" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B387" s="6"/>
     </row>
-    <row r="388">
+    <row r="388" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B388" s="6"/>
     </row>
-    <row r="389">
+    <row r="389" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B389" s="6"/>
     </row>
-    <row r="390">
+    <row r="390" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B390" s="6"/>
     </row>
-    <row r="391">
+    <row r="391" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B391" s="6"/>
     </row>
-    <row r="392">
+    <row r="392" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B392" s="6"/>
     </row>
-    <row r="393">
+    <row r="393" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B393" s="6"/>
     </row>
-    <row r="394">
+    <row r="394" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B394" s="6"/>
     </row>
-    <row r="395">
+    <row r="395" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B395" s="6"/>
     </row>
-    <row r="396">
+    <row r="396" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B396" s="6"/>
     </row>
-    <row r="397">
+    <row r="397" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B397" s="6"/>
     </row>
-    <row r="398">
+    <row r="398" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B398" s="6"/>
     </row>
-    <row r="399">
+    <row r="399" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B399" s="6"/>
     </row>
-    <row r="400">
+    <row r="400" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B400" s="6"/>
     </row>
-    <row r="401">
+    <row r="401" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B401" s="6"/>
     </row>
-    <row r="402">
+    <row r="402" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B402" s="6"/>
     </row>
-    <row r="403">
+    <row r="403" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B403" s="6"/>
     </row>
-    <row r="404">
+    <row r="404" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B404" s="6"/>
     </row>
-    <row r="405">
+    <row r="405" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B405" s="6"/>
     </row>
-    <row r="406">
+    <row r="406" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B406" s="6"/>
     </row>
-    <row r="407">
+    <row r="407" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B407" s="6"/>
     </row>
-    <row r="408">
+    <row r="408" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B408" s="6"/>
     </row>
-    <row r="409">
+    <row r="409" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B409" s="6"/>
     </row>
-    <row r="410">
+    <row r="410" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B410" s="6"/>
     </row>
-    <row r="411">
+    <row r="411" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B411" s="6"/>
     </row>
-    <row r="412">
+    <row r="412" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B412" s="6"/>
     </row>
-    <row r="413">
+    <row r="413" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B413" s="6"/>
     </row>
-    <row r="414">
+    <row r="414" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B414" s="6"/>
     </row>
-    <row r="415">
+    <row r="415" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B415" s="6"/>
     </row>
-    <row r="416">
+    <row r="416" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B416" s="6"/>
     </row>
-    <row r="417">
+    <row r="417" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B417" s="6"/>
     </row>
-    <row r="418">
+    <row r="418" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B418" s="6"/>
     </row>
-    <row r="419">
+    <row r="419" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B419" s="6"/>
     </row>
-    <row r="420">
+    <row r="420" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B420" s="6"/>
     </row>
-    <row r="421">
+    <row r="421" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B421" s="6"/>
     </row>
-    <row r="422">
+    <row r="422" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B422" s="6"/>
     </row>
-    <row r="423">
+    <row r="423" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B423" s="6"/>
     </row>
-    <row r="424">
+    <row r="424" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B424" s="6"/>
     </row>
-    <row r="425">
+    <row r="425" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B425" s="6"/>
     </row>
-    <row r="426">
+    <row r="426" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B426" s="6"/>
     </row>
-    <row r="427">
+    <row r="427" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B427" s="6"/>
     </row>
-    <row r="428">
+    <row r="428" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B428" s="6"/>
     </row>
-    <row r="429">
+    <row r="429" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B429" s="6"/>
     </row>
-    <row r="430">
+    <row r="430" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B430" s="6"/>
     </row>
-    <row r="431">
+    <row r="431" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B431" s="6"/>
     </row>
-    <row r="432">
+    <row r="432" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B432" s="6"/>
     </row>
-    <row r="433">
+    <row r="433" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B433" s="6"/>
     </row>
-    <row r="434">
+    <row r="434" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B434" s="6"/>
     </row>
-    <row r="435">
+    <row r="435" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B435" s="6"/>
     </row>
-    <row r="436">
+    <row r="436" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B436" s="6"/>
     </row>
-    <row r="437">
+    <row r="437" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B437" s="6"/>
     </row>
-    <row r="438">
+    <row r="438" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B438" s="6"/>
     </row>
-    <row r="439">
+    <row r="439" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B439" s="6"/>
     </row>
-    <row r="440">
+    <row r="440" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B440" s="6"/>
     </row>
-    <row r="441">
+    <row r="441" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B441" s="6"/>
     </row>
-    <row r="442">
+    <row r="442" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B442" s="6"/>
     </row>
-    <row r="443">
+    <row r="443" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B443" s="6"/>
     </row>
-    <row r="444">
+    <row r="444" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B444" s="6"/>
     </row>
-    <row r="445">
+    <row r="445" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B445" s="6"/>
     </row>
-    <row r="446">
+    <row r="446" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B446" s="6"/>
     </row>
-    <row r="447">
+    <row r="447" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B447" s="6"/>
     </row>
-    <row r="448">
+    <row r="448" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B448" s="6"/>
     </row>
-    <row r="449">
+    <row r="449" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B449" s="6"/>
     </row>
-    <row r="450">
+    <row r="450" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B450" s="6"/>
     </row>
-    <row r="451">
+    <row r="451" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B451" s="6"/>
     </row>
-    <row r="452">
+    <row r="452" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B452" s="6"/>
     </row>
-    <row r="453">
+    <row r="453" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B453" s="6"/>
     </row>
-    <row r="454">
+    <row r="454" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B454" s="6"/>
     </row>
-    <row r="455">
+    <row r="455" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B455" s="6"/>
     </row>
-    <row r="456">
+    <row r="456" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B456" s="6"/>
     </row>
-    <row r="457">
+    <row r="457" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B457" s="6"/>
     </row>
-    <row r="458">
+    <row r="458" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B458" s="6"/>
     </row>
-    <row r="459">
+    <row r="459" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B459" s="6"/>
     </row>
-    <row r="460">
+    <row r="460" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B460" s="6"/>
     </row>
-    <row r="461">
+    <row r="461" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B461" s="6"/>
     </row>
-    <row r="462">
+    <row r="462" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B462" s="6"/>
     </row>
-    <row r="463">
+    <row r="463" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B463" s="6"/>
     </row>
-    <row r="464">
+    <row r="464" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B464" s="6"/>
     </row>
-    <row r="465">
+    <row r="465" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B465" s="6"/>
     </row>
-    <row r="466">
+    <row r="466" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B466" s="6"/>
     </row>
-    <row r="467">
+    <row r="467" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B467" s="6"/>
     </row>
-    <row r="468">
+    <row r="468" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B468" s="6"/>
     </row>
-    <row r="469">
+    <row r="469" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B469" s="6"/>
     </row>
-    <row r="470">
+    <row r="470" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B470" s="6"/>
     </row>
-    <row r="471">
+    <row r="471" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B471" s="6"/>
     </row>
-    <row r="472">
+    <row r="472" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B472" s="6"/>
     </row>
-    <row r="473">
+    <row r="473" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B473" s="6"/>
     </row>
-    <row r="474">
+    <row r="474" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B474" s="6"/>
     </row>
-    <row r="475">
+    <row r="475" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B475" s="6"/>
     </row>
-    <row r="476">
+    <row r="476" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B476" s="6"/>
     </row>
-    <row r="477">
+    <row r="477" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B477" s="6"/>
     </row>
-    <row r="478">
+    <row r="478" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B478" s="6"/>
     </row>
-    <row r="479">
+    <row r="479" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B479" s="6"/>
     </row>
-    <row r="480">
+    <row r="480" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B480" s="6"/>
     </row>
-    <row r="481">
+    <row r="481" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B481" s="6"/>
     </row>
-    <row r="482">
+    <row r="482" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B482" s="6"/>
     </row>
-    <row r="483">
+    <row r="483" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B483" s="6"/>
     </row>
-    <row r="484">
+    <row r="484" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B484" s="6"/>
     </row>
-    <row r="485">
+    <row r="485" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B485" s="6"/>
     </row>
-    <row r="486">
+    <row r="486" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B486" s="6"/>
     </row>
-    <row r="487">
+    <row r="487" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B487" s="6"/>
     </row>
-    <row r="488">
+    <row r="488" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B488" s="6"/>
     </row>
-    <row r="489">
+    <row r="489" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B489" s="6"/>
     </row>
-    <row r="490">
+    <row r="490" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B490" s="6"/>
     </row>
-    <row r="491">
+    <row r="491" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B491" s="6"/>
     </row>
-    <row r="492">
+    <row r="492" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B492" s="6"/>
     </row>
-    <row r="493">
+    <row r="493" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B493" s="6"/>
     </row>
-    <row r="494">
+    <row r="494" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B494" s="6"/>
     </row>
-    <row r="495">
+    <row r="495" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B495" s="6"/>
     </row>
-    <row r="496">
+    <row r="496" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B496" s="6"/>
     </row>
-    <row r="497">
+    <row r="497" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B497" s="6"/>
     </row>
-    <row r="498">
+    <row r="498" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B498" s="6"/>
     </row>
-    <row r="499">
+    <row r="499" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B499" s="6"/>
     </row>
-    <row r="500">
+    <row r="500" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B500" s="6"/>
     </row>
-    <row r="501">
+    <row r="501" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B501" s="6"/>
     </row>
-    <row r="502">
+    <row r="502" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B502" s="6"/>
     </row>
-    <row r="503">
+    <row r="503" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B503" s="6"/>
     </row>
-    <row r="504">
+    <row r="504" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B504" s="6"/>
     </row>
-    <row r="505">
+    <row r="505" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B505" s="6"/>
     </row>
-    <row r="506">
+    <row r="506" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B506" s="6"/>
     </row>
-    <row r="507">
+    <row r="507" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B507" s="6"/>
     </row>
-    <row r="508">
+    <row r="508" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B508" s="6"/>
     </row>
-    <row r="509">
+    <row r="509" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B509" s="6"/>
     </row>
-    <row r="510">
+    <row r="510" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B510" s="6"/>
     </row>
-    <row r="511">
+    <row r="511" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B511" s="6"/>
     </row>
-    <row r="512">
+    <row r="512" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B512" s="6"/>
     </row>
-    <row r="513">
+    <row r="513" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B513" s="6"/>
     </row>
-    <row r="514">
+    <row r="514" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B514" s="6"/>
     </row>
-    <row r="515">
+    <row r="515" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B515" s="6"/>
     </row>
-    <row r="516">
+    <row r="516" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B516" s="6"/>
     </row>
-    <row r="517">
+    <row r="517" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B517" s="6"/>
     </row>
-    <row r="518">
+    <row r="518" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B518" s="6"/>
     </row>
-    <row r="519">
+    <row r="519" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B519" s="6"/>
     </row>
-    <row r="520">
+    <row r="520" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B520" s="6"/>
     </row>
-    <row r="521">
+    <row r="521" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B521" s="6"/>
     </row>
-    <row r="522">
+    <row r="522" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B522" s="6"/>
     </row>
-    <row r="523">
+    <row r="523" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B523" s="6"/>
     </row>
-    <row r="524">
+    <row r="524" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B524" s="6"/>
     </row>
-    <row r="525">
+    <row r="525" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B525" s="6"/>
     </row>
-    <row r="526">
+    <row r="526" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B526" s="6"/>
     </row>
-    <row r="527">
+    <row r="527" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B527" s="6"/>
     </row>
-    <row r="528">
+    <row r="528" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B528" s="6"/>
     </row>
-    <row r="529">
+    <row r="529" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B529" s="6"/>
     </row>
-    <row r="530">
+    <row r="530" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B530" s="6"/>
     </row>
-    <row r="531">
+    <row r="531" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B531" s="6"/>
     </row>
-    <row r="532">
+    <row r="532" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B532" s="6"/>
     </row>
-    <row r="533">
+    <row r="533" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B533" s="6"/>
     </row>
-    <row r="534">
+    <row r="534" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B534" s="6"/>
     </row>
-    <row r="535">
+    <row r="535" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B535" s="6"/>
     </row>
-    <row r="536">
+    <row r="536" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B536" s="6"/>
     </row>
-    <row r="537">
+    <row r="537" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B537" s="6"/>
     </row>
-    <row r="538">
+    <row r="538" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B538" s="6"/>
     </row>
-    <row r="539">
+    <row r="539" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B539" s="6"/>
     </row>
-    <row r="540">
+    <row r="540" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B540" s="6"/>
     </row>
-    <row r="541">
+    <row r="541" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B541" s="6"/>
     </row>
-    <row r="542">
+    <row r="542" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B542" s="6"/>
     </row>
-    <row r="543">
+    <row r="543" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B543" s="6"/>
     </row>
-    <row r="544">
+    <row r="544" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B544" s="6"/>
     </row>
-    <row r="545">
+    <row r="545" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B545" s="6"/>
     </row>
-    <row r="546">
+    <row r="546" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B546" s="6"/>
     </row>
-    <row r="547">
+    <row r="547" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B547" s="6"/>
     </row>
-    <row r="548">
+    <row r="548" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B548" s="6"/>
     </row>
-    <row r="549">
+    <row r="549" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B549" s="6"/>
     </row>
-    <row r="550">
+    <row r="550" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B550" s="6"/>
     </row>
-    <row r="551">
+    <row r="551" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B551" s="6"/>
     </row>
-    <row r="552">
+    <row r="552" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B552" s="6"/>
     </row>
-    <row r="553">
+    <row r="553" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B553" s="6"/>
     </row>
-    <row r="554">
+    <row r="554" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B554" s="6"/>
     </row>
-    <row r="555">
+    <row r="555" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B555" s="6"/>
     </row>
-    <row r="556">
+    <row r="556" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B556" s="6"/>
     </row>
-    <row r="557">
+    <row r="557" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B557" s="6"/>
     </row>
-    <row r="558">
+    <row r="558" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B558" s="6"/>
     </row>
-    <row r="559">
+    <row r="559" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B559" s="6"/>
     </row>
-    <row r="560">
+    <row r="560" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B560" s="6"/>
     </row>
-    <row r="561">
+    <row r="561" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B561" s="6"/>
     </row>
-    <row r="562">
+    <row r="562" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B562" s="6"/>
     </row>
-    <row r="563">
+    <row r="563" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B563" s="6"/>
     </row>
-    <row r="564">
+    <row r="564" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B564" s="6"/>
     </row>
-    <row r="565">
+    <row r="565" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B565" s="6"/>
     </row>
-    <row r="566">
+    <row r="566" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B566" s="6"/>
     </row>
-    <row r="567">
+    <row r="567" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B567" s="6"/>
     </row>
-    <row r="568">
+    <row r="568" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B568" s="6"/>
     </row>
-    <row r="569">
+    <row r="569" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B569" s="6"/>
     </row>
-    <row r="570">
+    <row r="570" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B570" s="6"/>
     </row>
-    <row r="571">
+    <row r="571" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B571" s="6"/>
     </row>
-    <row r="572">
+    <row r="572" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B572" s="6"/>
     </row>
-    <row r="573">
+    <row r="573" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B573" s="6"/>
     </row>
-    <row r="574">
+    <row r="574" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B574" s="6"/>
     </row>
-    <row r="575">
+    <row r="575" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B575" s="6"/>
     </row>
-    <row r="576">
+    <row r="576" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B576" s="6"/>
     </row>
-    <row r="577">
+    <row r="577" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B577" s="6"/>
     </row>
-    <row r="578">
+    <row r="578" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B578" s="6"/>
     </row>
-    <row r="579">
+    <row r="579" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B579" s="6"/>
     </row>
-    <row r="580">
+    <row r="580" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B580" s="6"/>
     </row>
-    <row r="581">
+    <row r="581" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B581" s="6"/>
     </row>
-    <row r="582">
+    <row r="582" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B582" s="6"/>
     </row>
-    <row r="583">
+    <row r="583" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B583" s="6"/>
     </row>
-    <row r="584">
+    <row r="584" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B584" s="6"/>
     </row>
-    <row r="585">
+    <row r="585" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B585" s="6"/>
     </row>
-    <row r="586">
+    <row r="586" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B586" s="6"/>
     </row>
-    <row r="587">
+    <row r="587" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B587" s="6"/>
     </row>
-    <row r="588">
+    <row r="588" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B588" s="6"/>
     </row>
-    <row r="589">
+    <row r="589" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B589" s="6"/>
     </row>
-    <row r="590">
+    <row r="590" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B590" s="6"/>
     </row>
-    <row r="591">
+    <row r="591" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B591" s="6"/>
     </row>
-    <row r="592">
+    <row r="592" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B592" s="6"/>
     </row>
-    <row r="593">
+    <row r="593" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B593" s="6"/>
     </row>
-    <row r="594">
+    <row r="594" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B594" s="6"/>
     </row>
-    <row r="595">
+    <row r="595" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B595" s="6"/>
     </row>
-    <row r="596">
+    <row r="596" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B596" s="6"/>
     </row>
-    <row r="597">
+    <row r="597" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B597" s="6"/>
     </row>
-    <row r="598">
+    <row r="598" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B598" s="6"/>
     </row>
-    <row r="599">
+    <row r="599" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B599" s="6"/>
     </row>
-    <row r="600">
+    <row r="600" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B600" s="6"/>
     </row>
-    <row r="601">
+    <row r="601" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B601" s="6"/>
     </row>
-    <row r="602">
+    <row r="602" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B602" s="6"/>
     </row>
-    <row r="603">
+    <row r="603" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B603" s="6"/>
     </row>
-    <row r="604">
+    <row r="604" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B604" s="6"/>
     </row>
-    <row r="605">
+    <row r="605" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B605" s="6"/>
     </row>
-    <row r="606">
+    <row r="606" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B606" s="6"/>
     </row>
-    <row r="607">
+    <row r="607" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B607" s="6"/>
     </row>
-    <row r="608">
+    <row r="608" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B608" s="6"/>
     </row>
-    <row r="609">
+    <row r="609" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B609" s="6"/>
     </row>
-    <row r="610">
+    <row r="610" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B610" s="6"/>
     </row>
-    <row r="611">
+    <row r="611" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B611" s="6"/>
     </row>
-    <row r="612">
+    <row r="612" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B612" s="6"/>
     </row>
-    <row r="613">
+    <row r="613" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B613" s="6"/>
     </row>
-    <row r="614">
+    <row r="614" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B614" s="6"/>
     </row>
-    <row r="615">
+    <row r="615" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B615" s="6"/>
     </row>
-    <row r="616">
+    <row r="616" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B616" s="6"/>
     </row>
-    <row r="617">
+    <row r="617" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B617" s="6"/>
     </row>
-    <row r="618">
+    <row r="618" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B618" s="6"/>
     </row>
-    <row r="619">
+    <row r="619" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B619" s="6"/>
     </row>
-    <row r="620">
+    <row r="620" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B620" s="6"/>
     </row>
-    <row r="621">
+    <row r="621" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B621" s="6"/>
     </row>
-    <row r="622">
+    <row r="622" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B622" s="6"/>
     </row>
-    <row r="623">
+    <row r="623" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B623" s="6"/>
     </row>
-    <row r="624">
+    <row r="624" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B624" s="6"/>
     </row>
-    <row r="625">
+    <row r="625" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B625" s="6"/>
     </row>
-    <row r="626">
+    <row r="626" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B626" s="6"/>
     </row>
-    <row r="627">
+    <row r="627" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B627" s="6"/>
     </row>
-    <row r="628">
+    <row r="628" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B628" s="6"/>
     </row>
-    <row r="629">
+    <row r="629" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B629" s="6"/>
     </row>
-    <row r="630">
+    <row r="630" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B630" s="6"/>
     </row>
-    <row r="631">
+    <row r="631" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B631" s="6"/>
     </row>
-    <row r="632">
+    <row r="632" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B632" s="6"/>
     </row>
-    <row r="633">
+    <row r="633" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B633" s="6"/>
     </row>
-    <row r="634">
+    <row r="634" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B634" s="6"/>
     </row>
-    <row r="635">
+    <row r="635" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B635" s="6"/>
     </row>
-    <row r="636">
+    <row r="636" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B636" s="6"/>
     </row>
-    <row r="637">
+    <row r="637" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B637" s="6"/>
     </row>
-    <row r="638">
+    <row r="638" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B638" s="6"/>
     </row>
-    <row r="639">
+    <row r="639" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B639" s="6"/>
     </row>
-    <row r="640">
+    <row r="640" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B640" s="6"/>
     </row>
-    <row r="641">
+    <row r="641" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B641" s="6"/>
     </row>
-    <row r="642">
+    <row r="642" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B642" s="6"/>
     </row>
-    <row r="643">
+    <row r="643" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B643" s="6"/>
     </row>
-    <row r="644">
+    <row r="644" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B644" s="6"/>
     </row>
-    <row r="645">
+    <row r="645" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B645" s="6"/>
     </row>
-    <row r="646">
+    <row r="646" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B646" s="6"/>
     </row>
-    <row r="647">
+    <row r="647" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B647" s="6"/>
     </row>
-    <row r="648">
+    <row r="648" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B648" s="6"/>
     </row>
-    <row r="649">
+    <row r="649" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B649" s="6"/>
     </row>
-    <row r="650">
+    <row r="650" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B650" s="6"/>
     </row>
-    <row r="651">
+    <row r="651" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B651" s="6"/>
     </row>
-    <row r="652">
+    <row r="652" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B652" s="6"/>
     </row>
-    <row r="653">
+    <row r="653" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B653" s="6"/>
     </row>
-    <row r="654">
+    <row r="654" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B654" s="6"/>
     </row>
-    <row r="655">
+    <row r="655" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B655" s="6"/>
     </row>
-    <row r="656">
+    <row r="656" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B656" s="6"/>
     </row>
-    <row r="657">
+    <row r="657" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B657" s="6"/>
     </row>
-    <row r="658">
+    <row r="658" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B658" s="6"/>
     </row>
-    <row r="659">
+    <row r="659" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B659" s="6"/>
     </row>
-    <row r="660">
+    <row r="660" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B660" s="6"/>
     </row>
-    <row r="661">
+    <row r="661" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B661" s="6"/>
     </row>
-    <row r="662">
+    <row r="662" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B662" s="6"/>
     </row>
-    <row r="663">
+    <row r="663" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B663" s="6"/>
     </row>
-    <row r="664">
+    <row r="664" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B664" s="6"/>
     </row>
-    <row r="665">
+    <row r="665" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B665" s="6"/>
     </row>
-    <row r="666">
+    <row r="666" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B666" s="6"/>
     </row>
-    <row r="667">
+    <row r="667" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B667" s="6"/>
     </row>
-    <row r="668">
+    <row r="668" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B668" s="6"/>
     </row>
-    <row r="669">
+    <row r="669" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B669" s="6"/>
     </row>
-    <row r="670">
+    <row r="670" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B670" s="6"/>
     </row>
-    <row r="671">
+    <row r="671" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B671" s="6"/>
     </row>
-    <row r="672">
+    <row r="672" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B672" s="6"/>
     </row>
-    <row r="673">
+    <row r="673" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B673" s="6"/>
     </row>
-    <row r="674">
+    <row r="674" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B674" s="6"/>
     </row>
-    <row r="675">
+    <row r="675" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B675" s="6"/>
     </row>
-    <row r="676">
+    <row r="676" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B676" s="6"/>
     </row>
-    <row r="677">
+    <row r="677" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B677" s="6"/>
     </row>
-    <row r="678">
+    <row r="678" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B678" s="6"/>
     </row>
-    <row r="679">
+    <row r="679" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B679" s="6"/>
     </row>
-    <row r="680">
+    <row r="680" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B680" s="6"/>
     </row>
-    <row r="681">
+    <row r="681" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B681" s="6"/>
     </row>
-    <row r="682">
+    <row r="682" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B682" s="6"/>
     </row>
-    <row r="683">
+    <row r="683" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B683" s="6"/>
     </row>
-    <row r="684">
+    <row r="684" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B684" s="6"/>
     </row>
-    <row r="685">
+    <row r="685" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B685" s="6"/>
     </row>
-    <row r="686">
+    <row r="686" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B686" s="6"/>
     </row>
-    <row r="687">
+    <row r="687" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B687" s="6"/>
     </row>
-    <row r="688">
+    <row r="688" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B688" s="6"/>
     </row>
-    <row r="689">
+    <row r="689" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B689" s="6"/>
     </row>
-    <row r="690">
+    <row r="690" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B690" s="6"/>
     </row>
-    <row r="691">
+    <row r="691" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B691" s="6"/>
     </row>
-    <row r="692">
+    <row r="692" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B692" s="6"/>
     </row>
-    <row r="693">
+    <row r="693" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B693" s="6"/>
     </row>
-    <row r="694">
+    <row r="694" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B694" s="6"/>
     </row>
-    <row r="695">
+    <row r="695" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B695" s="6"/>
     </row>
-    <row r="696">
+    <row r="696" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B696" s="6"/>
     </row>
-    <row r="697">
+    <row r="697" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B697" s="6"/>
     </row>
-    <row r="698">
+    <row r="698" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B698" s="6"/>
     </row>
-    <row r="699">
+    <row r="699" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B699" s="6"/>
     </row>
-    <row r="700">
+    <row r="700" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B700" s="6"/>
     </row>
-    <row r="701">
+    <row r="701" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B701" s="6"/>
     </row>
-    <row r="702">
+    <row r="702" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B702" s="6"/>
     </row>
-    <row r="703">
+    <row r="703" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B703" s="6"/>
     </row>
-    <row r="704">
+    <row r="704" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B704" s="6"/>
     </row>
-    <row r="705">
+    <row r="705" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B705" s="6"/>
     </row>
-    <row r="706">
+    <row r="706" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B706" s="6"/>
     </row>
-    <row r="707">
+    <row r="707" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B707" s="6"/>
     </row>
-    <row r="708">
+    <row r="708" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B708" s="6"/>
     </row>
-    <row r="709">
+    <row r="709" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B709" s="6"/>
     </row>
-    <row r="710">
+    <row r="710" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B710" s="6"/>
     </row>
-    <row r="711">
+    <row r="711" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B711" s="6"/>
     </row>
-    <row r="712">
+    <row r="712" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B712" s="6"/>
     </row>
-    <row r="713">
+    <row r="713" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B713" s="6"/>
     </row>
-    <row r="714">
+    <row r="714" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B714" s="6"/>
     </row>
-    <row r="715">
+    <row r="715" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B715" s="6"/>
     </row>
-    <row r="716">
+    <row r="716" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B716" s="6"/>
     </row>
-    <row r="717">
+    <row r="717" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B717" s="6"/>
     </row>
-    <row r="718">
+    <row r="718" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B718" s="6"/>
     </row>
-    <row r="719">
+    <row r="719" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B719" s="6"/>
     </row>
-    <row r="720">
+    <row r="720" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B720" s="6"/>
     </row>
-    <row r="721">
+    <row r="721" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B721" s="6"/>
     </row>
-    <row r="722">
+    <row r="722" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B722" s="6"/>
     </row>
-    <row r="723">
+    <row r="723" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B723" s="6"/>
     </row>
-    <row r="724">
+    <row r="724" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B724" s="6"/>
     </row>
-    <row r="725">
+    <row r="725" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B725" s="6"/>
     </row>
-    <row r="726">
+    <row r="726" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B726" s="6"/>
     </row>
-    <row r="727">
+    <row r="727" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B727" s="6"/>
     </row>
-    <row r="728">
+    <row r="728" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B728" s="6"/>
     </row>
-    <row r="729">
+    <row r="729" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B729" s="6"/>
     </row>
-    <row r="730">
+    <row r="730" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B730" s="6"/>
     </row>
-    <row r="731">
+    <row r="731" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B731" s="6"/>
     </row>
-    <row r="732">
+    <row r="732" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B732" s="6"/>
     </row>
-    <row r="733">
+    <row r="733" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B733" s="6"/>
     </row>
-    <row r="734">
+    <row r="734" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B734" s="6"/>
     </row>
-    <row r="735">
+    <row r="735" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B735" s="6"/>
     </row>
-    <row r="736">
+    <row r="736" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B736" s="6"/>
     </row>
-    <row r="737">
+    <row r="737" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B737" s="6"/>
     </row>
-    <row r="738">
+    <row r="738" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B738" s="6"/>
     </row>
-    <row r="739">
+    <row r="739" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B739" s="6"/>
     </row>
-    <row r="740">
+    <row r="740" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B740" s="6"/>
     </row>
-    <row r="741">
+    <row r="741" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B741" s="6"/>
     </row>
-    <row r="742">
+    <row r="742" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B742" s="6"/>
     </row>
-    <row r="743">
+    <row r="743" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B743" s="6"/>
     </row>
-    <row r="744">
+    <row r="744" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B744" s="6"/>
     </row>
-    <row r="745">
+    <row r="745" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B745" s="6"/>
     </row>
-    <row r="746">
+    <row r="746" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B746" s="6"/>
     </row>
-    <row r="747">
+    <row r="747" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B747" s="6"/>
     </row>
-    <row r="748">
+    <row r="748" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B748" s="6"/>
     </row>
-    <row r="749">
+    <row r="749" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B749" s="6"/>
     </row>
-    <row r="750">
+    <row r="750" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B750" s="6"/>
     </row>
-    <row r="751">
+    <row r="751" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B751" s="6"/>
     </row>
-    <row r="752">
+    <row r="752" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B752" s="6"/>
     </row>
-    <row r="753">
+    <row r="753" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B753" s="6"/>
     </row>
-    <row r="754">
+    <row r="754" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B754" s="6"/>
     </row>
-    <row r="755">
+    <row r="755" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B755" s="6"/>
     </row>
-    <row r="756">
+    <row r="756" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B756" s="6"/>
     </row>
-    <row r="757">
+    <row r="757" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B757" s="6"/>
     </row>
-    <row r="758">
+    <row r="758" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B758" s="6"/>
     </row>
-    <row r="759">
+    <row r="759" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B759" s="6"/>
     </row>
-    <row r="760">
+    <row r="760" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B760" s="6"/>
     </row>
-    <row r="761">
+    <row r="761" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B761" s="6"/>
     </row>
-    <row r="762">
+    <row r="762" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B762" s="6"/>
     </row>
-    <row r="763">
+    <row r="763" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B763" s="6"/>
     </row>
-    <row r="764">
+    <row r="764" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B764" s="6"/>
     </row>
-    <row r="765">
+    <row r="765" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B765" s="6"/>
     </row>
-    <row r="766">
+    <row r="766" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B766" s="6"/>
     </row>
-    <row r="767">
+    <row r="767" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B767" s="6"/>
     </row>
-    <row r="768">
+    <row r="768" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B768" s="6"/>
     </row>
-    <row r="769">
+    <row r="769" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B769" s="6"/>
     </row>
-    <row r="770">
+    <row r="770" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B770" s="6"/>
     </row>
-    <row r="771">
+    <row r="771" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B771" s="6"/>
     </row>
-    <row r="772">
+    <row r="772" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B772" s="6"/>
     </row>
-    <row r="773">
+    <row r="773" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B773" s="6"/>
     </row>
-    <row r="774">
+    <row r="774" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B774" s="6"/>
     </row>
-    <row r="775">
+    <row r="775" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B775" s="6"/>
     </row>
-    <row r="776">
+    <row r="776" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B776" s="6"/>
     </row>
-    <row r="777">
+    <row r="777" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B777" s="6"/>
     </row>
-    <row r="778">
+    <row r="778" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B778" s="6"/>
     </row>
-    <row r="779">
+    <row r="779" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B779" s="6"/>
     </row>
-    <row r="780">
+    <row r="780" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B780" s="6"/>
     </row>
-    <row r="781">
+    <row r="781" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B781" s="6"/>
     </row>
-    <row r="782">
+    <row r="782" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B782" s="6"/>
     </row>
-    <row r="783">
+    <row r="783" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B783" s="6"/>
     </row>
-    <row r="784">
+    <row r="784" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B784" s="6"/>
     </row>
-    <row r="785">
+    <row r="785" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B785" s="6"/>
     </row>
-    <row r="786">
+    <row r="786" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B786" s="6"/>
     </row>
-    <row r="787">
+    <row r="787" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B787" s="6"/>
     </row>
-    <row r="788">
+    <row r="788" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B788" s="6"/>
     </row>
-    <row r="789">
+    <row r="789" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B789" s="6"/>
     </row>
-    <row r="790">
+    <row r="790" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B790" s="6"/>
     </row>
-    <row r="791">
+    <row r="791" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B791" s="6"/>
     </row>
-    <row r="792">
+    <row r="792" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B792" s="6"/>
     </row>
-    <row r="793">
+    <row r="793" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B793" s="6"/>
     </row>
-    <row r="794">
+    <row r="794" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B794" s="6"/>
     </row>
-    <row r="795">
+    <row r="795" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B795" s="6"/>
     </row>
-    <row r="796">
+    <row r="796" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B796" s="6"/>
     </row>
-    <row r="797">
+    <row r="797" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B797" s="6"/>
     </row>
-    <row r="798">
+    <row r="798" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B798" s="6"/>
     </row>
-    <row r="799">
+    <row r="799" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B799" s="6"/>
     </row>
-    <row r="800">
+    <row r="800" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B800" s="6"/>
     </row>
-    <row r="801">
+    <row r="801" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B801" s="6"/>
     </row>
-    <row r="802">
+    <row r="802" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B802" s="6"/>
     </row>
-    <row r="803">
+    <row r="803" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B803" s="6"/>
     </row>
-    <row r="804">
+    <row r="804" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B804" s="6"/>
     </row>
-    <row r="805">
+    <row r="805" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B805" s="6"/>
     </row>
-    <row r="806">
+    <row r="806" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B806" s="6"/>
     </row>
-    <row r="807">
+    <row r="807" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B807" s="6"/>
     </row>
-    <row r="808">
+    <row r="808" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B808" s="6"/>
     </row>
-    <row r="809">
+    <row r="809" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B809" s="6"/>
     </row>
-    <row r="810">
+    <row r="810" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B810" s="6"/>
     </row>
-    <row r="811">
+    <row r="811" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B811" s="6"/>
     </row>
-    <row r="812">
+    <row r="812" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B812" s="6"/>
     </row>
-    <row r="813">
+    <row r="813" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B813" s="6"/>
     </row>
-    <row r="814">
+    <row r="814" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B814" s="6"/>
     </row>
-    <row r="815">
+    <row r="815" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B815" s="6"/>
     </row>
-    <row r="816">
+    <row r="816" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B816" s="6"/>
     </row>
-    <row r="817">
+    <row r="817" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B817" s="6"/>
     </row>
-    <row r="818">
+    <row r="818" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B818" s="6"/>
     </row>
-    <row r="819">
+    <row r="819" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B819" s="6"/>
     </row>
-    <row r="820">
+    <row r="820" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B820" s="6"/>
     </row>
-    <row r="821">
+    <row r="821" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B821" s="6"/>
     </row>
-    <row r="822">
+    <row r="822" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B822" s="6"/>
     </row>
-    <row r="823">
+    <row r="823" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B823" s="6"/>
     </row>
-    <row r="824">
+    <row r="824" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B824" s="6"/>
     </row>
-    <row r="825">
+    <row r="825" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B825" s="6"/>
     </row>
-    <row r="826">
+    <row r="826" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B826" s="6"/>
     </row>
-    <row r="827">
+    <row r="827" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B827" s="6"/>
     </row>
-    <row r="828">
+    <row r="828" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B828" s="6"/>
     </row>
-    <row r="829">
+    <row r="829" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B829" s="6"/>
     </row>
-    <row r="830">
+    <row r="830" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B830" s="6"/>
     </row>
-    <row r="831">
+    <row r="831" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B831" s="6"/>
     </row>
-    <row r="832">
+    <row r="832" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B832" s="6"/>
     </row>
-    <row r="833">
+    <row r="833" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B833" s="6"/>
     </row>
-    <row r="834">
+    <row r="834" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B834" s="6"/>
     </row>
-    <row r="835">
+    <row r="835" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B835" s="6"/>
     </row>
-    <row r="836">
+    <row r="836" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B836" s="6"/>
     </row>
-    <row r="837">
+    <row r="837" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B837" s="6"/>
     </row>
-    <row r="838">
+    <row r="838" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B838" s="6"/>
     </row>
-    <row r="839">
+    <row r="839" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B839" s="6"/>
     </row>
-    <row r="840">
+    <row r="840" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B840" s="6"/>
     </row>
-    <row r="841">
+    <row r="841" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B841" s="6"/>
     </row>
-    <row r="842">
+    <row r="842" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B842" s="6"/>
     </row>
-    <row r="843">
+    <row r="843" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B843" s="6"/>
     </row>
-    <row r="844">
+    <row r="844" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B844" s="6"/>
     </row>
-    <row r="845">
+    <row r="845" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B845" s="6"/>
     </row>
-    <row r="846">
+    <row r="846" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B846" s="6"/>
     </row>
-    <row r="847">
+    <row r="847" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B847" s="6"/>
     </row>
-    <row r="848">
+    <row r="848" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B848" s="6"/>
     </row>
-    <row r="849">
+    <row r="849" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B849" s="6"/>
     </row>
-    <row r="850">
+    <row r="850" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B850" s="6"/>
     </row>
-    <row r="851">
+    <row r="851" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B851" s="6"/>
     </row>
-    <row r="852">
+    <row r="852" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B852" s="6"/>
     </row>
-    <row r="853">
+    <row r="853" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B853" s="6"/>
     </row>
-    <row r="854">
+    <row r="854" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B854" s="6"/>
     </row>
-    <row r="855">
+    <row r="855" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B855" s="6"/>
     </row>
-    <row r="856">
+    <row r="856" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B856" s="6"/>
     </row>
-    <row r="857">
+    <row r="857" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B857" s="6"/>
     </row>
-    <row r="858">
+    <row r="858" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B858" s="6"/>
     </row>
-    <row r="859">
+    <row r="859" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B859" s="6"/>
     </row>
-    <row r="860">
+    <row r="860" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B860" s="6"/>
     </row>
-    <row r="861">
+    <row r="861" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B861" s="6"/>
     </row>
-    <row r="862">
+    <row r="862" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B862" s="6"/>
     </row>
-    <row r="863">
+    <row r="863" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B863" s="6"/>
     </row>
-    <row r="864">
+    <row r="864" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B864" s="6"/>
     </row>
-    <row r="865">
+    <row r="865" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B865" s="6"/>
     </row>
-    <row r="866">
+    <row r="866" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B866" s="6"/>
     </row>
-    <row r="867">
+    <row r="867" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B867" s="6"/>
     </row>
-    <row r="868">
+    <row r="868" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B868" s="6"/>
     </row>
-    <row r="869">
+    <row r="869" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B869" s="6"/>
     </row>
-    <row r="870">
+    <row r="870" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B870" s="6"/>
     </row>
-    <row r="871">
+    <row r="871" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B871" s="6"/>
     </row>
-    <row r="872">
+    <row r="872" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B872" s="6"/>
     </row>
-    <row r="873">
+    <row r="873" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B873" s="6"/>
     </row>
-    <row r="874">
+    <row r="874" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B874" s="6"/>
     </row>
-    <row r="875">
+    <row r="875" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B875" s="6"/>
     </row>
-    <row r="876">
+    <row r="876" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B876" s="6"/>
     </row>
-    <row r="877">
+    <row r="877" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B877" s="6"/>
     </row>
-    <row r="878">
+    <row r="878" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B878" s="6"/>
     </row>
-    <row r="879">
+    <row r="879" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B879" s="6"/>
     </row>
-    <row r="880">
+    <row r="880" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B880" s="6"/>
     </row>
-    <row r="881">
+    <row r="881" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B881" s="6"/>
     </row>
-    <row r="882">
+    <row r="882" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B882" s="6"/>
     </row>
-    <row r="883">
+    <row r="883" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B883" s="6"/>
     </row>
-    <row r="884">
+    <row r="884" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B884" s="6"/>
     </row>
-    <row r="885">
+    <row r="885" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B885" s="6"/>
     </row>
-    <row r="886">
+    <row r="886" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B886" s="6"/>
     </row>
-    <row r="887">
+    <row r="887" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B887" s="6"/>
     </row>
-    <row r="888">
+    <row r="888" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B888" s="6"/>
     </row>
-    <row r="889">
+    <row r="889" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B889" s="6"/>
     </row>
-    <row r="890">
+    <row r="890" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B890" s="6"/>
     </row>
-    <row r="891">
+    <row r="891" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B891" s="6"/>
     </row>
-    <row r="892">
+    <row r="892" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B892" s="6"/>
     </row>
-    <row r="893">
+    <row r="893" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B893" s="6"/>
     </row>
-    <row r="894">
+    <row r="894" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B894" s="6"/>
     </row>
-    <row r="895">
+    <row r="895" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B895" s="6"/>
     </row>
-    <row r="896">
+    <row r="896" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B896" s="6"/>
     </row>
-    <row r="897">
+    <row r="897" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B897" s="6"/>
     </row>
-    <row r="898">
+    <row r="898" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B898" s="6"/>
     </row>
-    <row r="899">
+    <row r="899" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B899" s="6"/>
     </row>
-    <row r="900">
+    <row r="900" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B900" s="6"/>
     </row>
-    <row r="901">
+    <row r="901" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B901" s="6"/>
     </row>
-    <row r="902">
+    <row r="902" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B902" s="6"/>
     </row>
-    <row r="903">
+    <row r="903" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B903" s="6"/>
     </row>
-    <row r="904">
+    <row r="904" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B904" s="6"/>
     </row>
-    <row r="905">
+    <row r="905" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B905" s="6"/>
     </row>
-    <row r="906">
+    <row r="906" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B906" s="6"/>
     </row>
-    <row r="907">
+    <row r="907" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B907" s="6"/>
     </row>
-    <row r="908">
+    <row r="908" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B908" s="6"/>
     </row>
-    <row r="909">
+    <row r="909" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B909" s="6"/>
     </row>
-    <row r="910">
+    <row r="910" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B910" s="6"/>
     </row>
-    <row r="911">
+    <row r="911" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B911" s="6"/>
     </row>
-    <row r="912">
+    <row r="912" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B912" s="6"/>
     </row>
-    <row r="913">
+    <row r="913" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B913" s="6"/>
     </row>
-    <row r="914">
+    <row r="914" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B914" s="6"/>
     </row>
-    <row r="915">
+    <row r="915" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B915" s="6"/>
     </row>
-    <row r="916">
+    <row r="916" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B916" s="6"/>
     </row>
-    <row r="917">
+    <row r="917" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B917" s="6"/>
     </row>
-    <row r="918">
+    <row r="918" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B918" s="6"/>
     </row>
-    <row r="919">
+    <row r="919" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B919" s="6"/>
     </row>
-    <row r="920">
+    <row r="920" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B920" s="6"/>
     </row>
-    <row r="921">
+    <row r="921" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B921" s="6"/>
     </row>
-    <row r="922">
+    <row r="922" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B922" s="6"/>
     </row>
-    <row r="923">
+    <row r="923" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B923" s="6"/>
     </row>
-    <row r="924">
+    <row r="924" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B924" s="6"/>
     </row>
-    <row r="925">
+    <row r="925" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B925" s="6"/>
     </row>
-    <row r="926">
+    <row r="926" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B926" s="6"/>
     </row>
-    <row r="927">
+    <row r="927" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B927" s="6"/>
     </row>
-    <row r="928">
+    <row r="928" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B928" s="6"/>
     </row>
-    <row r="929">
+    <row r="929" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B929" s="6"/>
     </row>
-    <row r="930">
+    <row r="930" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B930" s="6"/>
     </row>
-    <row r="931">
+    <row r="931" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B931" s="6"/>
     </row>
-    <row r="932">
+    <row r="932" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B932" s="6"/>
     </row>
-    <row r="933">
+    <row r="933" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B933" s="6"/>
     </row>
-    <row r="934">
+    <row r="934" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B934" s="6"/>
     </row>
-    <row r="935">
+    <row r="935" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B935" s="6"/>
     </row>
-    <row r="936">
+    <row r="936" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B936" s="6"/>
     </row>
-    <row r="937">
+    <row r="937" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B937" s="6"/>
     </row>
-    <row r="938">
+    <row r="938" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B938" s="6"/>
     </row>
-    <row r="939">
+    <row r="939" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B939" s="6"/>
     </row>
-    <row r="940">
+    <row r="940" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B940" s="6"/>
     </row>
-    <row r="941">
+    <row r="941" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B941" s="6"/>
     </row>
-    <row r="942">
+    <row r="942" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B942" s="6"/>
     </row>
-    <row r="943">
+    <row r="943" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B943" s="6"/>
     </row>
-    <row r="944">
+    <row r="944" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B944" s="6"/>
     </row>
-    <row r="945">
+    <row r="945" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B945" s="6"/>
     </row>
-    <row r="946">
+    <row r="946" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B946" s="6"/>
     </row>
-    <row r="947">
+    <row r="947" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B947" s="6"/>
     </row>
-    <row r="948">
+    <row r="948" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B948" s="6"/>
     </row>
-    <row r="949">
+    <row r="949" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B949" s="6"/>
     </row>
-    <row r="950">
+    <row r="950" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B950" s="6"/>
     </row>
-    <row r="951">
+    <row r="951" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B951" s="6"/>
     </row>
-    <row r="952">
+    <row r="952" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B952" s="6"/>
     </row>
-    <row r="953">
+    <row r="953" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B953" s="6"/>
     </row>
-    <row r="954">
+    <row r="954" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B954" s="6"/>
     </row>
-    <row r="955">
+    <row r="955" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B955" s="6"/>
     </row>
-    <row r="956">
+    <row r="956" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B956" s="6"/>
     </row>
-    <row r="957">
+    <row r="957" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B957" s="6"/>
     </row>
-    <row r="958">
+    <row r="958" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B958" s="6"/>
     </row>
-    <row r="959">
+    <row r="959" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B959" s="6"/>
     </row>
-    <row r="960">
+    <row r="960" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B960" s="6"/>
     </row>
-    <row r="961">
+    <row r="961" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B961" s="6"/>
     </row>
-    <row r="962">
+    <row r="962" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B962" s="6"/>
     </row>
-    <row r="963">
+    <row r="963" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B963" s="6"/>
     </row>
-    <row r="964">
+    <row r="964" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B964" s="6"/>
     </row>
-    <row r="965">
+    <row r="965" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B965" s="6"/>
     </row>
-    <row r="966">
+    <row r="966" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B966" s="6"/>
     </row>
-    <row r="967">
+    <row r="967" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B967" s="6"/>
     </row>
-    <row r="968">
+    <row r="968" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B968" s="6"/>
     </row>
-    <row r="969">
+    <row r="969" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B969" s="6"/>
     </row>
-    <row r="970">
+    <row r="970" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B970" s="6"/>
     </row>
-    <row r="971">
+    <row r="971" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B971" s="6"/>
     </row>
-    <row r="972">
+    <row r="972" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B972" s="6"/>
     </row>
-    <row r="973">
+    <row r="973" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B973" s="6"/>
     </row>
-    <row r="974">
+    <row r="974" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B974" s="6"/>
     </row>
-    <row r="975">
+    <row r="975" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B975" s="6"/>
     </row>
-    <row r="976">
+    <row r="976" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B976" s="6"/>
     </row>
-    <row r="977">
+    <row r="977" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B977" s="6"/>
     </row>
-    <row r="978">
+    <row r="978" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B978" s="6"/>
     </row>
-    <row r="979">
+    <row r="979" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B979" s="6"/>
     </row>
-    <row r="980">
+    <row r="980" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B980" s="6"/>
     </row>
-    <row r="981">
+    <row r="981" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B981" s="6"/>
     </row>
-    <row r="982">
+    <row r="982" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B982" s="6"/>
     </row>
-    <row r="983">
+    <row r="983" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B983" s="6"/>
     </row>
-    <row r="984">
+    <row r="984" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B984" s="6"/>
     </row>
-    <row r="985">
+    <row r="985" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B985" s="6"/>
     </row>
-    <row r="986">
+    <row r="986" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B986" s="6"/>
     </row>
-    <row r="987">
+    <row r="987" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B987" s="6"/>
     </row>
-    <row r="988">
+    <row r="988" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B988" s="6"/>
     </row>
-    <row r="989">
+    <row r="989" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B989" s="6"/>
     </row>
-    <row r="990">
+    <row r="990" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B990" s="6"/>
     </row>
-    <row r="991">
+    <row r="991" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B991" s="6"/>
     </row>
-    <row r="992">
+    <row r="992" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B992" s="6"/>
     </row>
-    <row r="993">
+    <row r="993" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B993" s="6"/>
     </row>
-    <row r="994">
+    <row r="994" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B994" s="6"/>
     </row>
-    <row r="995">
+    <row r="995" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B995" s="6"/>
     </row>
-    <row r="996">
+    <row r="996" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B996" s="6"/>
     </row>
-    <row r="997">
+    <row r="997" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B997" s="6"/>
     </row>
-    <row r="998">
+    <row r="998" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B998" s="6"/>
     </row>
-    <row r="999">
+    <row r="999" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B999" s="6"/>
     </row>
-    <row r="1000">
+    <row r="1000" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1000" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>